<commit_message>
fix - string less than 10 as yaml string
</commit_message>
<xml_diff>
--- a/tests/assets/testfileopenxml.xlsx
+++ b/tests/assets/testfileopenxml.xlsx
@@ -53,9 +53,6 @@
     <t>surname1</t>
   </si>
   <si>
-    <t>emailmycorp.com</t>
-  </si>
-  <si>
     <t>a text with some spaces</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>surname8</t>
+  </si>
+  <si>
+    <t>email@mycorp.com</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,18 +459,18 @@
         <v>666555444</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="1" t="d">
         <v>2025-11-29</v>
@@ -479,18 +479,18 @@
         <v>666555445</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="1" t="d">
         <v>2025-11-30</v>
@@ -499,18 +499,18 @@
         <v>666555446</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5" s="1" t="d">
         <v>2025-12-01</v>
@@ -519,18 +519,18 @@
         <v>666555447</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="1" t="d">
         <v>2025-12-02</v>
@@ -539,18 +539,18 @@
         <v>666555448</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="1" t="d">
         <v>2025-12-03</v>
@@ -559,18 +559,18 @@
         <v>666555449</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
       </c>
       <c r="C8" s="1" t="d">
         <v>2025-12-04</v>
@@ -579,18 +579,18 @@
         <v>666555450</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="1" t="d">
         <v>2025-12-05</v>
@@ -599,10 +599,10 @@
         <v>666555451</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>